<commit_message>
Now with data table
</commit_message>
<xml_diff>
--- a/brainstorm_clinic_data.xlsx
+++ b/brainstorm_clinic_data.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10705"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jenny/retriever/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E41AD3C1-355D-6A44-8D12-837E4C7D7196}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54254990-F813-1F40-B43C-FA56E4BDA883}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12800" yWindow="460" windowWidth="12800" windowHeight="14840" xr2:uid="{516412A6-7196-4648-9F28-0B1A58CCCA25}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14820" activeTab="1" xr2:uid="{516412A6-7196-4648-9F28-0B1A58CCCA25}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="54">
   <si>
     <t>Hosptial</t>
   </si>
@@ -189,6 +190,12 @@
   </si>
   <si>
     <t xml:space="preserve">Risk score </t>
+  </si>
+  <si>
+    <t>Consults per vet</t>
+  </si>
+  <si>
+    <t>Procedures per vet</t>
   </si>
 </sst>
 </file>
@@ -212,15 +219,33 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -228,13 +253,91 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -551,8 +654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7611DD2-5AF1-E848-A536-09838D686397}">
   <dimension ref="A1:AB32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1108,4 +1211,456 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE34AD3D-B929-7C49-885E-D3F8A713E1B4}">
+  <dimension ref="A1:Z5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="12">
+        <v>8</v>
+      </c>
+      <c r="C2" s="12"/>
+      <c r="D2" s="13">
+        <f>B2+(C2/2)</f>
+        <v>8</v>
+      </c>
+      <c r="E2" s="14">
+        <v>10</v>
+      </c>
+      <c r="F2" s="18">
+        <f>B2*1.5</f>
+        <v>12</v>
+      </c>
+      <c r="G2" s="18"/>
+      <c r="H2" s="19">
+        <f>F2+(G2/2)</f>
+        <v>12</v>
+      </c>
+      <c r="I2" s="20">
+        <f>1.5*E2</f>
+        <v>15</v>
+      </c>
+      <c r="J2" s="24">
+        <v>3</v>
+      </c>
+      <c r="K2" s="24">
+        <v>6</v>
+      </c>
+      <c r="L2" s="25">
+        <f>J2+(K2/2)</f>
+        <v>6</v>
+      </c>
+      <c r="M2" s="26">
+        <v>8</v>
+      </c>
+      <c r="N2" s="8">
+        <v>32</v>
+      </c>
+      <c r="O2">
+        <f>32*4</f>
+        <v>128</v>
+      </c>
+      <c r="P2" s="4">
+        <f>32*5</f>
+        <v>160</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>5</v>
+      </c>
+      <c r="R2">
+        <f>5*3</f>
+        <v>15</v>
+      </c>
+      <c r="S2" s="4">
+        <f>5*4</f>
+        <v>20</v>
+      </c>
+      <c r="T2" s="5">
+        <v>50</v>
+      </c>
+      <c r="U2">
+        <f>O2*(T2/100)</f>
+        <v>64</v>
+      </c>
+      <c r="V2">
+        <f>U2/32</f>
+        <v>2</v>
+      </c>
+      <c r="W2">
+        <f>R2*(T2/100)</f>
+        <v>7.5</v>
+      </c>
+      <c r="X2">
+        <f>W2/5</f>
+        <v>1.5</v>
+      </c>
+      <c r="Y2">
+        <f>V2+X2</f>
+        <v>3.5</v>
+      </c>
+      <c r="Z2">
+        <f>ROUNDUP(Y2,0)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="12">
+        <v>2</v>
+      </c>
+      <c r="C3" s="12">
+        <v>0</v>
+      </c>
+      <c r="D3" s="13">
+        <f t="shared" ref="D3:D5" si="0">B3+(C3/2)</f>
+        <v>2</v>
+      </c>
+      <c r="E3" s="14">
+        <v>3</v>
+      </c>
+      <c r="F3" s="18">
+        <v>3</v>
+      </c>
+      <c r="G3" s="18">
+        <v>0</v>
+      </c>
+      <c r="H3" s="19">
+        <f t="shared" ref="H3:H5" si="1">F3+(G3/2)</f>
+        <v>3</v>
+      </c>
+      <c r="I3" s="20">
+        <v>3</v>
+      </c>
+      <c r="J3" s="24">
+        <v>1</v>
+      </c>
+      <c r="K3" s="24">
+        <v>1</v>
+      </c>
+      <c r="L3" s="25">
+        <f t="shared" ref="L3:L5" si="2">J3+(K3/2)</f>
+        <v>1.5</v>
+      </c>
+      <c r="M3" s="26">
+        <v>3</v>
+      </c>
+      <c r="N3" s="8">
+        <v>32</v>
+      </c>
+      <c r="O3">
+        <v>32</v>
+      </c>
+      <c r="P3" s="4">
+        <f>32*2</f>
+        <v>64</v>
+      </c>
+      <c r="Q3" s="8">
+        <v>5</v>
+      </c>
+      <c r="R3">
+        <v>5</v>
+      </c>
+      <c r="S3" s="4">
+        <v>5</v>
+      </c>
+      <c r="T3" s="5">
+        <v>50</v>
+      </c>
+      <c r="U3">
+        <f t="shared" ref="U3:U5" si="3">O3*(T3/100)</f>
+        <v>16</v>
+      </c>
+      <c r="V3">
+        <f t="shared" ref="V3:V5" si="4">U3/32</f>
+        <v>0.5</v>
+      </c>
+      <c r="W3">
+        <f t="shared" ref="W3:W5" si="5">R3*(T3/100)</f>
+        <v>2.5</v>
+      </c>
+      <c r="X3">
+        <f t="shared" ref="X3:X5" si="6">W3/5</f>
+        <v>0.5</v>
+      </c>
+      <c r="Y3">
+        <f t="shared" ref="Y3:Y5" si="7">V3+X3</f>
+        <v>1</v>
+      </c>
+      <c r="Z3">
+        <f t="shared" ref="Z3:Z5" si="8">ROUNDUP(Y3,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="12">
+        <v>2</v>
+      </c>
+      <c r="C4" s="12">
+        <v>0</v>
+      </c>
+      <c r="D4" s="13">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E4" s="14">
+        <v>3</v>
+      </c>
+      <c r="F4" s="18">
+        <v>3</v>
+      </c>
+      <c r="G4" s="18">
+        <v>0</v>
+      </c>
+      <c r="H4" s="19">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="I4" s="20">
+        <v>3</v>
+      </c>
+      <c r="J4" s="24">
+        <v>1</v>
+      </c>
+      <c r="K4" s="24">
+        <v>0</v>
+      </c>
+      <c r="L4" s="25">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="M4" s="26">
+        <v>3</v>
+      </c>
+      <c r="N4" s="8">
+        <v>32</v>
+      </c>
+      <c r="O4">
+        <v>32</v>
+      </c>
+      <c r="P4" s="4">
+        <f>32*2</f>
+        <v>64</v>
+      </c>
+      <c r="Q4" s="8">
+        <v>5</v>
+      </c>
+      <c r="R4">
+        <v>5</v>
+      </c>
+      <c r="S4" s="4">
+        <v>5</v>
+      </c>
+      <c r="T4" s="5">
+        <v>50</v>
+      </c>
+      <c r="U4">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="V4">
+        <f t="shared" si="4"/>
+        <v>0.5</v>
+      </c>
+      <c r="W4">
+        <f t="shared" si="5"/>
+        <v>2.5</v>
+      </c>
+      <c r="X4">
+        <f t="shared" si="6"/>
+        <v>0.5</v>
+      </c>
+      <c r="Y4">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="Z4">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="12">
+        <v>1</v>
+      </c>
+      <c r="C5" s="12">
+        <v>0</v>
+      </c>
+      <c r="D5" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E5" s="14">
+        <v>2</v>
+      </c>
+      <c r="F5" s="18">
+        <v>0</v>
+      </c>
+      <c r="G5" s="18">
+        <v>0</v>
+      </c>
+      <c r="H5" s="19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I5" s="20">
+        <v>1</v>
+      </c>
+      <c r="J5" s="24">
+        <v>1</v>
+      </c>
+      <c r="K5" s="24">
+        <v>0</v>
+      </c>
+      <c r="L5" s="25">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="M5" s="26">
+        <v>3</v>
+      </c>
+      <c r="N5" s="8">
+        <v>32</v>
+      </c>
+      <c r="O5">
+        <v>32</v>
+      </c>
+      <c r="P5" s="4">
+        <v>32</v>
+      </c>
+      <c r="Q5" s="8">
+        <v>5</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5" s="4">
+        <v>0</v>
+      </c>
+      <c r="T5" s="5">
+        <v>50</v>
+      </c>
+      <c r="U5">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="V5">
+        <f t="shared" si="4"/>
+        <v>0.5</v>
+      </c>
+      <c r="W5">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y5">
+        <f t="shared" si="7"/>
+        <v>0.5</v>
+      </c>
+      <c r="Z5">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
New warning and map
New warning & map
</commit_message>
<xml_diff>
--- a/brainstorm_clinic_data.xlsx
+++ b/brainstorm_clinic_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jenny/retriever/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54254990-F813-1F40-B43C-FA56E4BDA883}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C6B7341-5DED-0844-A114-DB46088ABC46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14820" activeTab="1" xr2:uid="{516412A6-7196-4648-9F28-0B1A58CCCA25}"/>
+    <workbookView xWindow="12800" yWindow="460" windowWidth="12800" windowHeight="14820" xr2:uid="{516412A6-7196-4648-9F28-0B1A58CCCA25}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="73">
   <si>
     <t>Hosptial</t>
   </si>
@@ -196,6 +196,63 @@
   </si>
   <si>
     <t>Procedures per vet</t>
+  </si>
+  <si>
+    <t>Consulting</t>
+  </si>
+  <si>
+    <t>Procedures</t>
+  </si>
+  <si>
+    <t>Other roles</t>
+  </si>
+  <si>
+    <t>Vet total</t>
+  </si>
+  <si>
+    <t>Vet req p</t>
+  </si>
+  <si>
+    <t>Vet req c</t>
+  </si>
+  <si>
+    <t>Vet rounded</t>
+  </si>
+  <si>
+    <t>Nurse req</t>
+  </si>
+  <si>
+    <t>Nurse rounded</t>
+  </si>
+  <si>
+    <t>Excess vets</t>
+  </si>
+  <si>
+    <t>Excess nurses</t>
+  </si>
+  <si>
+    <t>Possible consults</t>
+  </si>
+  <si>
+    <t>Routine Vets</t>
+  </si>
+  <si>
+    <t>Routine nurses</t>
+  </si>
+  <si>
+    <t>Possible Procedures</t>
+  </si>
+  <si>
+    <t>Caseload</t>
+  </si>
+  <si>
+    <t>Routine caseload</t>
+  </si>
+  <si>
+    <t>Caseload reduction</t>
+  </si>
+  <si>
+    <t>Nurse impact</t>
   </si>
 </sst>
 </file>
@@ -310,7 +367,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -338,6 +395,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -654,8 +712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7611DD2-5AF1-E848-A536-09838D686397}">
   <dimension ref="A1:AB32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1215,92 +1273,134 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE34AD3D-B929-7C49-885E-D3F8A713E1B4}">
-  <dimension ref="A1:Z5"/>
+  <dimension ref="A1:AN7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:40" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B1" s="9" t="s">
         <v>4</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="I1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="J1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="K1" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="L1" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="M1" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="N1" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="O1" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="P1" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="22" t="s">
+      <c r="Q1" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="23" t="s">
+      <c r="R1" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="U1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="X1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="Y1" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="V1" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="W1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="X1" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y1" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="Z1" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AD1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="AF1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AG1" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AI1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ1" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AK1" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AL1" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AM1" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AN1" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1308,90 +1408,141 @@
         <v>8</v>
       </c>
       <c r="C2" s="12"/>
-      <c r="D2" s="13">
+      <c r="D2" s="12">
+        <v>4</v>
+      </c>
+      <c r="E2" s="12">
+        <v>3</v>
+      </c>
+      <c r="F2" s="12">
+        <v>1</v>
+      </c>
+      <c r="G2" s="13">
+        <v>8</v>
+      </c>
+      <c r="H2" s="13">
         <f>B2+(C2/2)</f>
         <v>8</v>
       </c>
-      <c r="E2" s="14">
+      <c r="I2" s="14">
         <v>10</v>
       </c>
-      <c r="F2" s="18">
+      <c r="J2" s="18">
         <f>B2*1.5</f>
         <v>12</v>
       </c>
-      <c r="G2" s="18"/>
-      <c r="H2" s="19">
-        <f>F2+(G2/2)</f>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18">
         <v>12</v>
       </c>
-      <c r="I2" s="20">
-        <f>1.5*E2</f>
+      <c r="M2" s="19">
+        <f>J2+(K2/2)</f>
+        <v>12</v>
+      </c>
+      <c r="N2" s="20">
+        <f>1.5*I2</f>
         <v>15</v>
       </c>
-      <c r="J2" s="24">
-        <v>3</v>
-      </c>
-      <c r="K2" s="24">
+      <c r="O2" s="24">
+        <v>3</v>
+      </c>
+      <c r="P2" s="24">
         <v>6</v>
       </c>
-      <c r="L2" s="25">
-        <f>J2+(K2/2)</f>
+      <c r="Q2" s="25">
+        <f>O2+(P2/2)</f>
         <v>6</v>
       </c>
-      <c r="M2" s="26">
+      <c r="R2" s="26">
         <v>8</v>
       </c>
-      <c r="N2" s="8">
+      <c r="S2" s="8">
         <v>32</v>
       </c>
-      <c r="O2">
+      <c r="T2">
         <f>32*4</f>
         <v>128</v>
       </c>
-      <c r="P2" s="4">
+      <c r="U2" s="4">
         <f>32*5</f>
         <v>160</v>
       </c>
-      <c r="Q2" s="2">
+      <c r="V2" s="2">
         <v>5</v>
       </c>
-      <c r="R2">
+      <c r="W2">
         <f>5*3</f>
         <v>15</v>
       </c>
-      <c r="S2" s="4">
+      <c r="X2" s="4">
         <f>5*4</f>
         <v>20</v>
       </c>
-      <c r="T2" s="5">
+      <c r="Y2" s="4">
+        <f>T2+W2</f>
+        <v>143</v>
+      </c>
+      <c r="Z2" s="5">
         <v>50</v>
       </c>
-      <c r="U2">
-        <f>O2*(T2/100)</f>
+      <c r="AA2">
+        <f>T2*(Z2/100)</f>
         <v>64</v>
       </c>
-      <c r="V2">
-        <f>U2/32</f>
-        <v>2</v>
-      </c>
-      <c r="W2">
-        <f>R2*(T2/100)</f>
+      <c r="AB2">
+        <f>AA2/32</f>
+        <v>2</v>
+      </c>
+      <c r="AC2">
+        <f>W2*(Z2/100)</f>
         <v>7.5</v>
       </c>
-      <c r="X2">
-        <f>W2/5</f>
+      <c r="AD2">
+        <f>AC2/5</f>
         <v>1.5</v>
       </c>
-      <c r="Y2">
-        <f>V2+X2</f>
+      <c r="AE2">
+        <f>AB2+AD2</f>
         <v>3.5</v>
       </c>
-      <c r="Z2">
-        <f>ROUNDUP(Y2,0)</f>
+      <c r="AF2">
+        <f>ROUNDUP(AE2,0)</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AG2">
+        <f>AF2*1.5</f>
+        <v>6</v>
+      </c>
+      <c r="AH2">
+        <f>ROUNDUP(AG2,0)</f>
+        <v>6</v>
+      </c>
+      <c r="AI2">
+        <f>H2-AF2</f>
+        <v>4</v>
+      </c>
+      <c r="AJ2" s="4">
+        <f>M2-AH2</f>
+        <v>6</v>
+      </c>
+      <c r="AK2">
+        <f>S2*D2</f>
+        <v>128</v>
+      </c>
+      <c r="AL2">
+        <f>E2*V2</f>
+        <v>15</v>
+      </c>
+      <c r="AM2">
+        <f>AL2+AK2</f>
+        <v>143</v>
+      </c>
+      <c r="AN2">
+        <f>ROUNDUP((H2*1.5), 0)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1401,87 +1552,136 @@
       <c r="C3" s="12">
         <v>0</v>
       </c>
-      <c r="D3" s="13">
-        <f t="shared" ref="D3:D5" si="0">B3+(C3/2)</f>
-        <v>2</v>
-      </c>
-      <c r="E3" s="14">
-        <v>3</v>
-      </c>
-      <c r="F3" s="18">
-        <v>3</v>
-      </c>
-      <c r="G3" s="18">
-        <v>0</v>
-      </c>
-      <c r="H3" s="19">
-        <f t="shared" ref="H3:H5" si="1">F3+(G3/2)</f>
-        <v>3</v>
-      </c>
-      <c r="I3" s="20">
-        <v>3</v>
-      </c>
-      <c r="J3" s="24">
-        <v>1</v>
-      </c>
-      <c r="K3" s="24">
-        <v>1</v>
-      </c>
-      <c r="L3" s="25">
-        <f t="shared" ref="L3:L5" si="2">J3+(K3/2)</f>
+      <c r="D3" s="12">
+        <v>1</v>
+      </c>
+      <c r="E3" s="12">
+        <v>1</v>
+      </c>
+      <c r="F3" s="12"/>
+      <c r="G3" s="13">
+        <v>2</v>
+      </c>
+      <c r="H3" s="13">
+        <f>B3+(C3/2)</f>
+        <v>2</v>
+      </c>
+      <c r="I3" s="14">
+        <v>3</v>
+      </c>
+      <c r="J3" s="18">
+        <v>4</v>
+      </c>
+      <c r="K3" s="18">
+        <v>0</v>
+      </c>
+      <c r="L3" s="18">
+        <v>4</v>
+      </c>
+      <c r="M3" s="19">
+        <f t="shared" ref="M3:M5" si="0">J3+(K3/2)</f>
+        <v>4</v>
+      </c>
+      <c r="N3" s="20">
+        <v>3</v>
+      </c>
+      <c r="O3" s="24">
+        <v>1</v>
+      </c>
+      <c r="P3" s="24">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="25">
+        <f t="shared" ref="Q3:Q5" si="1">O3+(P3/2)</f>
         <v>1.5</v>
       </c>
-      <c r="M3" s="26">
-        <v>3</v>
-      </c>
-      <c r="N3" s="8">
+      <c r="R3" s="26">
+        <v>3</v>
+      </c>
+      <c r="S3" s="8">
         <v>32</v>
       </c>
-      <c r="O3">
+      <c r="T3">
         <v>32</v>
       </c>
-      <c r="P3" s="4">
+      <c r="U3" s="4">
         <f>32*2</f>
         <v>64</v>
       </c>
-      <c r="Q3" s="8">
+      <c r="V3" s="8">
         <v>5</v>
       </c>
-      <c r="R3">
+      <c r="W3">
         <v>5</v>
       </c>
-      <c r="S3" s="4">
+      <c r="X3" s="4">
         <v>5</v>
       </c>
-      <c r="T3" s="5">
+      <c r="Y3" s="4">
+        <f t="shared" ref="Y3:Y5" si="2">T3+W3</f>
+        <v>37</v>
+      </c>
+      <c r="Z3" s="5">
         <v>50</v>
       </c>
-      <c r="U3">
-        <f t="shared" ref="U3:U5" si="3">O3*(T3/100)</f>
+      <c r="AA3">
+        <f t="shared" ref="AA3:AA5" si="3">T3*(Z3/100)</f>
         <v>16</v>
       </c>
-      <c r="V3">
-        <f t="shared" ref="V3:V5" si="4">U3/32</f>
+      <c r="AB3">
+        <f t="shared" ref="AB3:AB5" si="4">AA3/32</f>
         <v>0.5</v>
       </c>
-      <c r="W3">
-        <f t="shared" ref="W3:W5" si="5">R3*(T3/100)</f>
+      <c r="AC3">
+        <f t="shared" ref="AC3:AC5" si="5">W3*(Z3/100)</f>
         <v>2.5</v>
       </c>
-      <c r="X3">
-        <f t="shared" ref="X3:X5" si="6">W3/5</f>
+      <c r="AD3">
+        <f t="shared" ref="AD3:AD5" si="6">AC3/5</f>
         <v>0.5</v>
       </c>
-      <c r="Y3">
-        <f t="shared" ref="Y3:Y5" si="7">V3+X3</f>
-        <v>1</v>
-      </c>
-      <c r="Z3">
-        <f t="shared" ref="Z3:Z5" si="8">ROUNDUP(Y3,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AE3">
+        <f t="shared" ref="AE3:AE5" si="7">AB3+AD3</f>
+        <v>1</v>
+      </c>
+      <c r="AF3">
+        <f t="shared" ref="AF3:AF5" si="8">ROUNDUP(AE3,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AG3">
+        <f t="shared" ref="AG3:AG5" si="9">AF3*1.5</f>
+        <v>1.5</v>
+      </c>
+      <c r="AH3">
+        <f t="shared" ref="AH3:AH5" si="10">ROUNDUP(AG3,0)</f>
+        <v>2</v>
+      </c>
+      <c r="AI3">
+        <f t="shared" ref="AI3:AI5" si="11">H3-AF3</f>
+        <v>1</v>
+      </c>
+      <c r="AJ3" s="4">
+        <f t="shared" ref="AJ3:AJ5" si="12">M3-AH3</f>
+        <v>2</v>
+      </c>
+      <c r="AK3">
+        <f t="shared" ref="AK3:AK5" si="13">S3*D3</f>
+        <v>32</v>
+      </c>
+      <c r="AL3">
+        <f t="shared" ref="AL3:AL5" si="14">E3*V3</f>
+        <v>5</v>
+      </c>
+      <c r="AM3">
+        <f t="shared" ref="AM3:AM5" si="15">AL3+AK3</f>
+        <v>37</v>
+      </c>
+      <c r="AN3">
+        <f t="shared" ref="AN3:AN5" si="16">ROUNDUP((H3*1.5), 0)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1491,87 +1691,136 @@
       <c r="C4" s="12">
         <v>0</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D4" s="12">
+        <v>1</v>
+      </c>
+      <c r="E4" s="12">
+        <v>1</v>
+      </c>
+      <c r="F4" s="12"/>
+      <c r="G4" s="13">
+        <v>2</v>
+      </c>
+      <c r="H4" s="13">
+        <f>B4+(C4/2)</f>
+        <v>2</v>
+      </c>
+      <c r="I4" s="14">
+        <v>3</v>
+      </c>
+      <c r="J4" s="18">
+        <v>4</v>
+      </c>
+      <c r="K4" s="18">
+        <v>0</v>
+      </c>
+      <c r="L4" s="18">
+        <v>4</v>
+      </c>
+      <c r="M4" s="19">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E4" s="14">
-        <v>3</v>
-      </c>
-      <c r="F4" s="18">
-        <v>3</v>
-      </c>
-      <c r="G4" s="18">
-        <v>0</v>
-      </c>
-      <c r="H4" s="19">
+        <v>4</v>
+      </c>
+      <c r="N4" s="20">
+        <v>3</v>
+      </c>
+      <c r="O4" s="24">
+        <v>1</v>
+      </c>
+      <c r="P4" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="25">
         <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="I4" s="20">
-        <v>3</v>
-      </c>
-      <c r="J4" s="24">
-        <v>1</v>
-      </c>
-      <c r="K4" s="24">
-        <v>0</v>
-      </c>
-      <c r="L4" s="25">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="M4" s="26">
-        <v>3</v>
-      </c>
-      <c r="N4" s="8">
+        <v>1</v>
+      </c>
+      <c r="R4" s="26">
+        <v>3</v>
+      </c>
+      <c r="S4" s="8">
         <v>32</v>
       </c>
-      <c r="O4">
+      <c r="T4">
         <v>32</v>
       </c>
-      <c r="P4" s="4">
+      <c r="U4" s="4">
         <f>32*2</f>
         <v>64</v>
       </c>
-      <c r="Q4" s="8">
+      <c r="V4" s="8">
         <v>5</v>
       </c>
-      <c r="R4">
+      <c r="W4">
         <v>5</v>
       </c>
-      <c r="S4" s="4">
+      <c r="X4" s="4">
         <v>5</v>
       </c>
-      <c r="T4" s="5">
+      <c r="Y4" s="4">
+        <f t="shared" si="2"/>
+        <v>37</v>
+      </c>
+      <c r="Z4" s="5">
         <v>50</v>
       </c>
-      <c r="U4">
+      <c r="AA4">
         <f t="shared" si="3"/>
         <v>16</v>
       </c>
-      <c r="V4">
+      <c r="AB4">
         <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
-      <c r="W4">
+      <c r="AC4">
         <f t="shared" si="5"/>
         <v>2.5</v>
       </c>
-      <c r="X4">
+      <c r="AD4">
         <f t="shared" si="6"/>
         <v>0.5</v>
       </c>
-      <c r="Y4">
+      <c r="AE4">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="Z4">
+      <c r="AF4">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AG4">
+        <f t="shared" si="9"/>
+        <v>1.5</v>
+      </c>
+      <c r="AH4">
+        <f t="shared" si="10"/>
+        <v>2</v>
+      </c>
+      <c r="AI4">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="AJ4" s="4">
+        <f t="shared" si="12"/>
+        <v>2</v>
+      </c>
+      <c r="AK4">
+        <f t="shared" si="13"/>
+        <v>32</v>
+      </c>
+      <c r="AL4">
+        <f t="shared" si="14"/>
+        <v>5</v>
+      </c>
+      <c r="AM4">
+        <f t="shared" si="15"/>
+        <v>37</v>
+      </c>
+      <c r="AN4">
+        <f t="shared" si="16"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1581,83 +1830,169 @@
       <c r="C5" s="12">
         <v>0</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="12">
+        <v>1</v>
+      </c>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="13">
+        <v>1</v>
+      </c>
+      <c r="H5" s="13">
+        <f>B5+(C5/2)</f>
+        <v>1</v>
+      </c>
+      <c r="I5" s="14">
+        <v>2</v>
+      </c>
+      <c r="J5" s="18">
+        <v>0</v>
+      </c>
+      <c r="K5" s="18">
+        <v>0</v>
+      </c>
+      <c r="L5" s="18">
+        <v>0</v>
+      </c>
+      <c r="M5" s="19">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E5" s="14">
-        <v>2</v>
-      </c>
-      <c r="F5" s="18">
-        <v>0</v>
-      </c>
-      <c r="G5" s="18">
-        <v>0</v>
-      </c>
-      <c r="H5" s="19">
+        <v>0</v>
+      </c>
+      <c r="N5" s="20">
+        <v>1</v>
+      </c>
+      <c r="O5" s="24">
+        <v>1</v>
+      </c>
+      <c r="P5" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="25">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I5" s="20">
-        <v>1</v>
-      </c>
-      <c r="J5" s="24">
-        <v>1</v>
-      </c>
-      <c r="K5" s="24">
-        <v>0</v>
-      </c>
-      <c r="L5" s="25">
+        <v>1</v>
+      </c>
+      <c r="R5" s="26">
+        <v>3</v>
+      </c>
+      <c r="S5" s="8">
+        <v>32</v>
+      </c>
+      <c r="T5">
+        <v>32</v>
+      </c>
+      <c r="U5" s="4">
+        <v>32</v>
+      </c>
+      <c r="V5" s="8">
+        <v>5</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="X5" s="4">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="4">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="M5" s="26">
-        <v>3</v>
-      </c>
-      <c r="N5" s="8">
         <v>32</v>
       </c>
-      <c r="O5">
-        <v>32</v>
-      </c>
-      <c r="P5" s="4">
-        <v>32</v>
-      </c>
-      <c r="Q5" s="8">
-        <v>5</v>
-      </c>
-      <c r="R5">
-        <v>0</v>
-      </c>
-      <c r="S5" s="4">
-        <v>0</v>
-      </c>
-      <c r="T5" s="5">
+      <c r="Z5" s="5">
         <v>50</v>
       </c>
-      <c r="U5">
+      <c r="AA5">
         <f t="shared" si="3"/>
         <v>16</v>
       </c>
-      <c r="V5">
+      <c r="AB5">
         <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
-      <c r="W5">
+      <c r="AC5">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="X5">
+      <c r="AD5">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="Y5">
+      <c r="AE5">
         <f t="shared" si="7"/>
         <v>0.5</v>
       </c>
-      <c r="Z5">
+      <c r="AF5">
         <f t="shared" si="8"/>
         <v>1</v>
+      </c>
+      <c r="AG5">
+        <f>AF5*1.5</f>
+        <v>1.5</v>
+      </c>
+      <c r="AH5">
+        <f>ROUNDUP(AG5,0)</f>
+        <v>2</v>
+      </c>
+      <c r="AI5">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AJ5" s="4">
+        <f t="shared" si="12"/>
+        <v>-2</v>
+      </c>
+      <c r="AK5">
+        <f t="shared" si="13"/>
+        <v>32</v>
+      </c>
+      <c r="AL5">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AM5">
+        <f t="shared" si="15"/>
+        <v>32</v>
+      </c>
+      <c r="AN5">
+        <f t="shared" si="16"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="M6" s="19">
+        <f>SUM(M2:M5)</f>
+        <v>20</v>
+      </c>
+      <c r="Y6" s="27">
+        <f>SUM(Y2:Y5)</f>
+        <v>249</v>
+      </c>
+      <c r="AI6">
+        <f>SUM(AI2:AI5)</f>
+        <v>6</v>
+      </c>
+      <c r="AJ6">
+        <f>SUM(AJ2:AJ5)</f>
+        <v>8</v>
+      </c>
+      <c r="AM6">
+        <f>SUM(AM2:AM5)</f>
+        <v>249</v>
+      </c>
+      <c r="AN6">
+        <f>SUM(AN2:AN5)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="AL7" t="s">
+        <v>71</v>
+      </c>
+      <c r="AM7">
+        <f>(AM6/Y6)*100</f>
+        <v>100</v>
+      </c>
+      <c r="AN7">
+        <f>M6-AN6</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>